<commit_message>
Update individual delta estimates
</commit_message>
<xml_diff>
--- a/Misc/Delta_Individual_Estimates.xlsx
+++ b/Misc/Delta_Individual_Estimates.xlsx
@@ -5,19 +5,17 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jorda\OneDrive - University of Tennessee\VPC\Misc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jorda\Documents\GitHub\VPC\Misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{95D5668B-8F28-4F8F-85BA-4CD01826EC47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF368E78-A216-4E22-8687-DB4B899520AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{660BBDA3-78F1-466A-B893-49A65C04D429}"/>
+    <workbookView xWindow="13980" yWindow="2595" windowWidth="12150" windowHeight="11835" xr2:uid="{660BBDA3-78F1-466A-B893-49A65C04D429}"/>
   </bookViews>
   <sheets>
     <sheet name="δ" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -61,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="8">
   <si>
     <t>VOLUNTEER</t>
   </si>
@@ -83,11 +81,17 @@
   <si>
     <t>δ</t>
   </si>
+  <si>
+    <t>Day</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -159,7 +163,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -169,6 +173,8 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -450,10 +456,10 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>δ!$B$5:$B$9</c:f>
+              <c:f>δ!$B$5:$B$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>3</c:v>
                 </c:pt>
@@ -465,19 +471,16 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>δ!$D$5:$D$9</c:f>
+              <c:f>δ!$D$5:$D$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>5.8713785102277276</c:v>
                 </c:pt>
@@ -489,9 +492,6 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>5.1967949799182538</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2.4533183400470375</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1038,20 +1038,17 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>δ!$B$76:$B$79</c:f>
+              <c:f>(δ!$B$76,δ!$B$78,δ!$B$79)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
                   <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
@@ -1059,20 +1056,17 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>δ!$D$76:$D$79</c:f>
+              <c:f>(δ!$D$76,δ!$D$78,δ!$D$79)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>6.4900145546065566</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.5051499783199058</c:v>
+                  <c:v>7.2797764390576933</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.2797764390576933</c:v>
-                </c:pt>
-                <c:pt idx="3">
                   <c:v>4.4737788346467244</c:v>
                 </c:pt>
               </c:numCache>
@@ -1620,23 +1614,17 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>δ!$B$84:$B$88</c:f>
+              <c:f>δ!$B$86:$B$88</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="4">
                   <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
@@ -1644,23 +1632,17 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>δ!$D$84:$D$88</c:f>
+              <c:f>δ!$D$86:$D$88</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>6.463650701501817</c:v>
+                  <c:v>5.3902142158386654</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.5358129375388927</c:v>
+                  <c:v>5.2000922826321068</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.3902142158386654</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5.2000922826321068</c:v>
-                </c:pt>
-                <c:pt idx="4">
                   <c:v>5.1090551886051667</c:v>
                 </c:pt>
               </c:numCache>
@@ -14269,825 +14251,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <xxl21:alternateUrls>
-      <xxl21:absoluteUrl r:id="rId2"/>
-    </xxl21:alternateUrls>
-    <sheetNames>
-      <sheetName val="Sheet1"/>
-      <sheetName val="Sheet2"/>
-      <sheetName val="Sheet3"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2">
-        <row r="2">
-          <cell r="A2">
-            <v>103</v>
-          </cell>
-          <cell r="B2">
-            <v>0</v>
-          </cell>
-          <cell r="D2">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="B3">
-            <v>1</v>
-          </cell>
-          <cell r="D3">
-            <v>3.8239304551255637</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="B4">
-            <v>2</v>
-          </cell>
-          <cell r="D4">
-            <v>5.3948245236591408</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="B5">
-            <v>3</v>
-          </cell>
-          <cell r="D5">
-            <v>5.8713785102277276</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="B6">
-            <v>4</v>
-          </cell>
-          <cell r="D6">
-            <v>5.122291258697234</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="B7">
-            <v>5</v>
-          </cell>
-          <cell r="D7">
-            <v>4.1605585621075578</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="B8">
-            <v>6</v>
-          </cell>
-          <cell r="D8">
-            <v>5.1967949799182538</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="B9">
-            <v>7</v>
-          </cell>
-          <cell r="D9">
-            <v>2.4533183400470375</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="A10">
-            <v>107</v>
-          </cell>
-          <cell r="B10">
-            <v>0</v>
-          </cell>
-          <cell r="D10">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="B11">
-            <v>1</v>
-          </cell>
-          <cell r="D11">
-            <v>3.1667260555800518</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="B12">
-            <v>2</v>
-          </cell>
-          <cell r="D12">
-            <v>4.7028611705729295</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="B13">
-            <v>3</v>
-          </cell>
-          <cell r="D13">
-            <v>5.4446255496991531</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="B14">
-            <v>4</v>
-          </cell>
-          <cell r="D14">
-            <v>6.5217025611528463</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="B15">
-            <v>5</v>
-          </cell>
-          <cell r="D15">
-            <v>5.7117355434534565</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="B16">
-            <v>6</v>
-          </cell>
-          <cell r="D16">
-            <v>4.3848728944929212</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="B17">
-            <v>7</v>
-          </cell>
-          <cell r="D17">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="A18">
-            <v>110</v>
-          </cell>
-          <cell r="B18">
-            <v>0</v>
-          </cell>
-          <cell r="D18">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="B19">
-            <v>1</v>
-          </cell>
-          <cell r="D19">
-            <v>3.8239304551255637</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="B20">
-            <v>2</v>
-          </cell>
-          <cell r="D20">
-            <v>5.2335113705749565</v>
-          </cell>
-        </row>
-        <row r="21">
-          <cell r="B21">
-            <v>3</v>
-          </cell>
-          <cell r="D21">
-            <v>5.2518376824661352</v>
-          </cell>
-        </row>
-        <row r="22">
-          <cell r="B22">
-            <v>4</v>
-          </cell>
-        </row>
-        <row r="23">
-          <cell r="B23">
-            <v>5</v>
-          </cell>
-          <cell r="D23">
-            <v>3.9674543681827408</v>
-          </cell>
-        </row>
-        <row r="24">
-          <cell r="B24">
-            <v>6</v>
-          </cell>
-          <cell r="D24">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="25">
-          <cell r="B25">
-            <v>7</v>
-          </cell>
-          <cell r="D25">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="26">
-          <cell r="A26">
-            <v>111</v>
-          </cell>
-          <cell r="B26">
-            <v>0</v>
-          </cell>
-          <cell r="D26">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="27">
-          <cell r="B27">
-            <v>1</v>
-          </cell>
-          <cell r="D27">
-            <v>3.8239304551255637</v>
-          </cell>
-        </row>
-        <row r="28">
-          <cell r="B28">
-            <v>2</v>
-          </cell>
-          <cell r="D28">
-            <v>5.2335113705749565</v>
-          </cell>
-        </row>
-        <row r="29">
-          <cell r="B29">
-            <v>3</v>
-          </cell>
-          <cell r="D29">
-            <v>5.442365300922031</v>
-          </cell>
-        </row>
-        <row r="30">
-          <cell r="B30">
-            <v>4</v>
-          </cell>
-          <cell r="D30">
-            <v>4.7160868537748319</v>
-          </cell>
-        </row>
-        <row r="31">
-          <cell r="B31">
-            <v>5</v>
-          </cell>
-          <cell r="D31">
-            <v>5.7763226454454557</v>
-          </cell>
-        </row>
-        <row r="32">
-          <cell r="B32">
-            <v>6</v>
-          </cell>
-          <cell r="D32">
-            <v>5.2234492122042315</v>
-          </cell>
-        </row>
-        <row r="33">
-          <cell r="B33">
-            <v>7</v>
-          </cell>
-          <cell r="D33">
-            <v>3.9049858810993632</v>
-          </cell>
-        </row>
-        <row r="34">
-          <cell r="A34">
-            <v>112</v>
-          </cell>
-          <cell r="B34">
-            <v>0</v>
-          </cell>
-          <cell r="D34">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="35">
-          <cell r="B35">
-            <v>1</v>
-          </cell>
-          <cell r="D35">
-            <v>3.8239304551255637</v>
-          </cell>
-        </row>
-        <row r="36">
-          <cell r="B36">
-            <v>2</v>
-          </cell>
-          <cell r="D36">
-            <v>5.2335113705749565</v>
-          </cell>
-        </row>
-        <row r="37">
-          <cell r="B37">
-            <v>3</v>
-          </cell>
-          <cell r="D37">
-            <v>5.8956092635736077</v>
-          </cell>
-        </row>
-        <row r="38">
-          <cell r="B38">
-            <v>4</v>
-          </cell>
-          <cell r="D38">
-            <v>6.1454441040410508</v>
-          </cell>
-        </row>
-        <row r="39">
-          <cell r="B39">
-            <v>5</v>
-          </cell>
-          <cell r="D39">
-            <v>2.4533183400470375</v>
-          </cell>
-        </row>
-        <row r="40">
-          <cell r="B40">
-            <v>6</v>
-          </cell>
-          <cell r="D40">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="41">
-          <cell r="B41">
-            <v>7</v>
-          </cell>
-        </row>
-        <row r="42">
-          <cell r="A42">
-            <v>204</v>
-          </cell>
-          <cell r="B42">
-            <v>0</v>
-          </cell>
-          <cell r="D42">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="43">
-          <cell r="B43">
-            <v>1</v>
-          </cell>
-          <cell r="D43">
-            <v>3.8239304551255637</v>
-          </cell>
-        </row>
-        <row r="44">
-          <cell r="B44">
-            <v>2</v>
-          </cell>
-          <cell r="D44">
-            <v>4.7454885801411457</v>
-          </cell>
-        </row>
-        <row r="45">
-          <cell r="B45">
-            <v>3</v>
-          </cell>
-          <cell r="D45">
-            <v>3.197831693328903</v>
-          </cell>
-        </row>
-        <row r="46">
-          <cell r="B46">
-            <v>4</v>
-          </cell>
-          <cell r="D46">
-            <v>2.9344984512435679</v>
-          </cell>
-        </row>
-        <row r="47">
-          <cell r="B47">
-            <v>5</v>
-          </cell>
-          <cell r="D47">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="48">
-          <cell r="B48">
-            <v>6</v>
-          </cell>
-          <cell r="D48">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="49">
-          <cell r="B49">
-            <v>7</v>
-          </cell>
-          <cell r="D49">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="50">
-          <cell r="A50">
-            <v>207</v>
-          </cell>
-          <cell r="B50">
-            <v>0</v>
-          </cell>
-          <cell r="D50">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="51">
-          <cell r="B51">
-            <v>1</v>
-          </cell>
-          <cell r="D51">
-            <v>3.8239304551255637</v>
-          </cell>
-        </row>
-        <row r="52">
-          <cell r="B52">
-            <v>2</v>
-          </cell>
-          <cell r="D52">
-            <v>5.7576761039599962</v>
-          </cell>
-        </row>
-        <row r="53">
-          <cell r="B53">
-            <v>3</v>
-          </cell>
-          <cell r="D53">
-            <v>6.2640360979047482</v>
-          </cell>
-        </row>
-        <row r="54">
-          <cell r="B54">
-            <v>4</v>
-          </cell>
-          <cell r="D54">
-            <v>4.7736621341582177</v>
-          </cell>
-        </row>
-        <row r="55">
-          <cell r="B55">
-            <v>5</v>
-          </cell>
-          <cell r="D55">
-            <v>2.6720978579357175</v>
-          </cell>
-        </row>
-        <row r="56">
-          <cell r="B56">
-            <v>6</v>
-          </cell>
-          <cell r="D56">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="57">
-          <cell r="B57">
-            <v>7</v>
-          </cell>
-          <cell r="D57">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="58">
-          <cell r="A58">
-            <v>301</v>
-          </cell>
-          <cell r="B58">
-            <v>0</v>
-          </cell>
-          <cell r="D58">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="59">
-          <cell r="B59">
-            <v>1</v>
-          </cell>
-          <cell r="D59">
-            <v>3.9679222067305173</v>
-          </cell>
-        </row>
-        <row r="60">
-          <cell r="B60">
-            <v>2</v>
-          </cell>
-          <cell r="D60">
-            <v>7.0053674077344672</v>
-          </cell>
-        </row>
-        <row r="61">
-          <cell r="B61">
-            <v>3</v>
-          </cell>
-          <cell r="D61">
-            <v>8.1666500947376388</v>
-          </cell>
-        </row>
-        <row r="62">
-          <cell r="B62">
-            <v>4</v>
-          </cell>
-          <cell r="D62">
-            <v>5.987829764784073</v>
-          </cell>
-        </row>
-        <row r="63">
-          <cell r="B63">
-            <v>5</v>
-          </cell>
-          <cell r="D63">
-            <v>6.3328388362158412</v>
-          </cell>
-        </row>
-        <row r="64">
-          <cell r="B64">
-            <v>6</v>
-          </cell>
-          <cell r="D64">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="65">
-          <cell r="B65">
-            <v>7</v>
-          </cell>
-          <cell r="D65">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="66">
-          <cell r="A66">
-            <v>302</v>
-          </cell>
-          <cell r="B66">
-            <v>0</v>
-          </cell>
-          <cell r="D66">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="67">
-          <cell r="B67">
-            <v>1</v>
-          </cell>
-          <cell r="D67">
-            <v>4.2565734381237244</v>
-          </cell>
-        </row>
-        <row r="68">
-          <cell r="B68">
-            <v>2</v>
-          </cell>
-          <cell r="D68">
-            <v>7.3333171278763789</v>
-          </cell>
-        </row>
-        <row r="69">
-          <cell r="B69">
-            <v>3</v>
-          </cell>
-          <cell r="D69">
-            <v>6.3489991789145153</v>
-          </cell>
-        </row>
-        <row r="70">
-          <cell r="B70">
-            <v>4</v>
-          </cell>
-          <cell r="D70">
-            <v>5.726229073683454</v>
-          </cell>
-        </row>
-        <row r="71">
-          <cell r="B71">
-            <v>5</v>
-          </cell>
-          <cell r="D71">
-            <v>5.239754811505569</v>
-          </cell>
-        </row>
-        <row r="72">
-          <cell r="B72">
-            <v>6</v>
-          </cell>
-          <cell r="D72">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="73">
-          <cell r="B73">
-            <v>7</v>
-          </cell>
-          <cell r="D73">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="74">
-          <cell r="A74">
-            <v>307</v>
-          </cell>
-          <cell r="B74">
-            <v>0</v>
-          </cell>
-          <cell r="D74">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="75">
-          <cell r="B75">
-            <v>1</v>
-          </cell>
-          <cell r="D75">
-            <v>4.9743366501461832</v>
-          </cell>
-        </row>
-        <row r="76">
-          <cell r="B76">
-            <v>2</v>
-          </cell>
-          <cell r="D76">
-            <v>6.4900145546065566</v>
-          </cell>
-        </row>
-        <row r="77">
-          <cell r="B77">
-            <v>3</v>
-          </cell>
-          <cell r="D77">
-            <v>3.5051499783199058</v>
-          </cell>
-        </row>
-        <row r="78">
-          <cell r="B78">
-            <v>4</v>
-          </cell>
-          <cell r="D78">
-            <v>7.2797764390576933</v>
-          </cell>
-        </row>
-        <row r="79">
-          <cell r="B79">
-            <v>5</v>
-          </cell>
-          <cell r="D79">
-            <v>4.4737788346467244</v>
-          </cell>
-        </row>
-        <row r="80">
-          <cell r="B80">
-            <v>6</v>
-          </cell>
-          <cell r="D80">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="81">
-          <cell r="B81">
-            <v>7</v>
-          </cell>
-          <cell r="D81">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="82">
-          <cell r="A82">
-            <v>308</v>
-          </cell>
-          <cell r="B82">
-            <v>0</v>
-          </cell>
-          <cell r="D82">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="83">
-          <cell r="B83">
-            <v>1</v>
-          </cell>
-          <cell r="D83">
-            <v>3.4163075870598827</v>
-          </cell>
-        </row>
-        <row r="84">
-          <cell r="B84">
-            <v>2</v>
-          </cell>
-          <cell r="D84">
-            <v>6.463650701501817</v>
-          </cell>
-        </row>
-        <row r="85">
-          <cell r="B85">
-            <v>3</v>
-          </cell>
-          <cell r="D85">
-            <v>4.5358129375388927</v>
-          </cell>
-        </row>
-        <row r="86">
-          <cell r="B86">
-            <v>4</v>
-          </cell>
-          <cell r="D86">
-            <v>5.3902142158386654</v>
-          </cell>
-        </row>
-        <row r="87">
-          <cell r="B87">
-            <v>5</v>
-          </cell>
-          <cell r="D87">
-            <v>5.2000922826321068</v>
-          </cell>
-        </row>
-        <row r="88">
-          <cell r="B88">
-            <v>6</v>
-          </cell>
-          <cell r="D88">
-            <v>5.1090551886051667</v>
-          </cell>
-        </row>
-        <row r="89">
-          <cell r="B89">
-            <v>7</v>
-          </cell>
-          <cell r="D89">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="90">
-          <cell r="A90">
-            <v>312</v>
-          </cell>
-          <cell r="B90">
-            <v>0</v>
-          </cell>
-          <cell r="D90">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="91">
-          <cell r="B91">
-            <v>1</v>
-          </cell>
-          <cell r="D91">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="92">
-          <cell r="B92">
-            <v>2</v>
-          </cell>
-          <cell r="D92">
-            <v>3.2260841159758238</v>
-          </cell>
-        </row>
-        <row r="93">
-          <cell r="B93">
-            <v>3</v>
-          </cell>
-          <cell r="D93">
-            <v>3.8442285813016279</v>
-          </cell>
-        </row>
-        <row r="94">
-          <cell r="B94">
-            <v>4</v>
-          </cell>
-          <cell r="D94">
-            <v>6.4570294197307767</v>
-          </cell>
-        </row>
-        <row r="95">
-          <cell r="B95">
-            <v>5</v>
-          </cell>
-          <cell r="D95">
-            <v>6.1351686024721932</v>
-          </cell>
-        </row>
-        <row r="96">
-          <cell r="B96">
-            <v>6</v>
-          </cell>
-          <cell r="D96">
-            <v>4.8373232356474141</v>
-          </cell>
-        </row>
-        <row r="97">
-          <cell r="B97">
-            <v>7</v>
-          </cell>
-          <cell r="D97">
-            <v>1</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -15407,8 +14570,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36985D2A-8E3F-4C08-B816-7EE32E3C5FF0}">
   <dimension ref="A1:Z97"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Y12" sqref="Y12"/>
+    <sheetView tabSelected="1" topLeftCell="P2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T17" sqref="T17:V19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15784,7 +14947,7 @@
         <v>4.3848728944929212</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>107</v>
       </c>
@@ -15797,8 +14960,17 @@
       <c r="D17">
         <v>1</v>
       </c>
+      <c r="T17" t="s">
+        <v>4</v>
+      </c>
+      <c r="U17" t="s">
+        <v>5</v>
+      </c>
+      <c r="V17" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>110</v>
       </c>
@@ -15811,8 +14983,18 @@
       <c r="D18">
         <v>1</v>
       </c>
+      <c r="T18">
+        <v>307</v>
+      </c>
+      <c r="U18" s="5">
+        <v>-0.22739999999999999</v>
+      </c>
+      <c r="V18" s="5">
+        <f t="shared" ref="V18" si="2">-U18*LN(10)</f>
+        <v>0.52360785014684597</v>
+      </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>110</v>
       </c>
@@ -15826,8 +15008,18 @@
         <f t="shared" si="0"/>
         <v>3.8239304551255637</v>
       </c>
+      <c r="T19">
+        <v>307</v>
+      </c>
+      <c r="U19" s="5">
+        <v>-0.51970000000000005</v>
+      </c>
+      <c r="V19" s="5">
+        <f t="shared" ref="V18:V19" si="3">-U19*LN(10)</f>
+        <v>1.1966534728290057</v>
+      </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>110</v>
       </c>
@@ -15842,7 +15034,7 @@
         <v>5.2335113705749565</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>110</v>
       </c>
@@ -15857,7 +15049,7 @@
         <v>5.2518376824661352</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>110</v>
       </c>
@@ -15865,7 +15057,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>110</v>
       </c>
@@ -15880,7 +15072,7 @@
         <v>3.9674543681827408</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>110</v>
       </c>
@@ -15894,7 +15086,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>110</v>
       </c>
@@ -15907,8 +15099,17 @@
       <c r="D25">
         <v>1</v>
       </c>
+      <c r="U25" t="s">
+        <v>4</v>
+      </c>
+      <c r="V25" t="s">
+        <v>7</v>
+      </c>
+      <c r="W25" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>111</v>
       </c>
@@ -15921,8 +15122,17 @@
       <c r="D26">
         <v>1</v>
       </c>
+      <c r="U26">
+        <v>112</v>
+      </c>
+      <c r="V26">
+        <v>0</v>
+      </c>
+      <c r="W26">
+        <v>0</v>
+      </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>111</v>
       </c>
@@ -15936,8 +15146,17 @@
         <f t="shared" si="0"/>
         <v>3.8239304551255637</v>
       </c>
+      <c r="U27">
+        <v>112</v>
+      </c>
+      <c r="V27">
+        <v>1</v>
+      </c>
+      <c r="W27" s="3">
+        <v>6667</v>
+      </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>111</v>
       </c>
@@ -15951,8 +15170,17 @@
         <f t="shared" si="0"/>
         <v>5.2335113705749565</v>
       </c>
+      <c r="U28">
+        <v>112</v>
+      </c>
+      <c r="V28">
+        <v>2</v>
+      </c>
+      <c r="W28" s="3">
+        <v>171203</v>
+      </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>111</v>
       </c>
@@ -15966,8 +15194,17 @@
         <f t="shared" si="0"/>
         <v>5.442365300922031</v>
       </c>
+      <c r="U29">
+        <v>112</v>
+      </c>
+      <c r="V29">
+        <v>3</v>
+      </c>
+      <c r="W29">
+        <v>786338</v>
+      </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>111</v>
       </c>
@@ -15981,8 +15218,17 @@
         <f t="shared" si="0"/>
         <v>4.7160868537748319</v>
       </c>
+      <c r="U30">
+        <v>112</v>
+      </c>
+      <c r="V30">
+        <v>4</v>
+      </c>
+      <c r="W30">
+        <v>1397797</v>
+      </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>111</v>
       </c>
@@ -15996,8 +15242,17 @@
         <f t="shared" si="0"/>
         <v>5.7763226454454557</v>
       </c>
+      <c r="U31">
+        <v>112</v>
+      </c>
+      <c r="V31">
+        <v>5</v>
+      </c>
+      <c r="W31">
+        <v>284</v>
+      </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>111</v>
       </c>
@@ -16011,8 +15266,17 @@
         <f t="shared" si="0"/>
         <v>5.2234492122042315</v>
       </c>
+      <c r="U32">
+        <v>112</v>
+      </c>
+      <c r="V32">
+        <v>6</v>
+      </c>
+      <c r="W32">
+        <v>0</v>
+      </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>111</v>
       </c>
@@ -16026,8 +15290,17 @@
         <f t="shared" si="0"/>
         <v>3.9049858810993632</v>
       </c>
+      <c r="U33">
+        <v>112</v>
+      </c>
+      <c r="V33">
+        <v>7</v>
+      </c>
+      <c r="W33">
+        <v>0</v>
+      </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>112</v>
       </c>
@@ -16041,7 +15314,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>112</v>
       </c>
@@ -16056,7 +15329,7 @@
         <v>3.8239304551255637</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>112</v>
       </c>
@@ -16071,7 +15344,7 @@
         <v>5.2335113705749565</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>112</v>
       </c>
@@ -16086,7 +15359,7 @@
         <v>5.8956092635736077</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>112</v>
       </c>
@@ -16101,7 +15374,7 @@
         <v>6.1454441040410508</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>112</v>
       </c>
@@ -16116,7 +15389,7 @@
         <v>2.4533183400470375</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>112</v>
       </c>
@@ -16130,7 +15403,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>112</v>
       </c>
@@ -16144,7 +15417,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>204</v>
       </c>
@@ -16158,7 +15431,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>204</v>
       </c>
@@ -16173,7 +15446,7 @@
         <v>3.8239304551255637</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>204</v>
       </c>
@@ -16188,7 +15461,7 @@
         <v>4.7454885801411457</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>204</v>
       </c>
@@ -16203,7 +15476,7 @@
         <v>3.197831693328903</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>204</v>
       </c>
@@ -16218,7 +15491,7 @@
         <v>2.9344984512435679</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>204</v>
       </c>
@@ -16232,7 +15505,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>204</v>
       </c>
@@ -16402,7 +15675,7 @@
         <v>9288</v>
       </c>
       <c r="D59">
-        <f t="shared" ref="D59:D96" si="2">LOG10(C59)</f>
+        <f t="shared" ref="D59:D96" si="4">LOG10(C59)</f>
         <v>3.9679222067305173</v>
       </c>
     </row>
@@ -16417,7 +15690,7 @@
         <v>10124356</v>
       </c>
       <c r="D60">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>7.0053674077344672</v>
       </c>
     </row>
@@ -16432,7 +15705,7 @@
         <v>146774326</v>
       </c>
       <c r="D61">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>8.1666500947376388</v>
       </c>
     </row>
@@ -16447,7 +15720,7 @@
         <v>972366</v>
       </c>
       <c r="D62">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>5.987829764784073</v>
       </c>
     </row>
@@ -16462,7 +15735,7 @@
         <v>2151983</v>
       </c>
       <c r="D63">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>6.3328388362158412</v>
       </c>
     </row>
@@ -16519,7 +15792,7 @@
         <v>18054</v>
       </c>
       <c r="D67">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4.2565734381237244</v>
       </c>
     </row>
@@ -16534,7 +15807,7 @@
         <v>21543543</v>
       </c>
       <c r="D68">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>7.3333171278763789</v>
       </c>
     </row>
@@ -16549,7 +15822,7 @@
         <v>2233568</v>
       </c>
       <c r="D69">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>6.3489991789145153</v>
       </c>
     </row>
@@ -16564,7 +15837,7 @@
         <v>532389</v>
       </c>
       <c r="D70">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>5.726229073683454</v>
       </c>
     </row>
@@ -16579,7 +15852,7 @@
         <v>173682</v>
       </c>
       <c r="D71">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>5.239754811505569</v>
       </c>
     </row>
@@ -16636,7 +15909,7 @@
         <v>94262</v>
       </c>
       <c r="D75">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4.9743366501461832</v>
       </c>
     </row>
@@ -16651,7 +15924,7 @@
         <v>3090399</v>
       </c>
       <c r="D76">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>6.4900145546065566</v>
       </c>
     </row>
@@ -16666,7 +15939,7 @@
         <v>3200</v>
       </c>
       <c r="D77">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3.5051499783199058</v>
       </c>
     </row>
@@ -16681,7 +15954,7 @@
         <v>19044801</v>
       </c>
       <c r="D78">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>7.2797764390576933</v>
       </c>
     </row>
@@ -16696,7 +15969,7 @@
         <v>29770</v>
       </c>
       <c r="D79">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4.4737788346467244</v>
       </c>
     </row>
@@ -16753,7 +16026,7 @@
         <v>2608</v>
       </c>
       <c r="D83">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3.4163075870598827</v>
       </c>
     </row>
@@ -16768,7 +16041,7 @@
         <v>2908377</v>
       </c>
       <c r="D84">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>6.463650701501817</v>
       </c>
     </row>
@@ -16783,7 +16056,7 @@
         <v>34341</v>
       </c>
       <c r="D85">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4.5358129375388927</v>
       </c>
     </row>
@@ -16798,7 +16071,7 @@
         <v>245592</v>
       </c>
       <c r="D86">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>5.3902142158386654</v>
       </c>
     </row>
@@ -16813,7 +16086,7 @@
         <v>158523</v>
       </c>
       <c r="D87">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>5.2000922826321068</v>
       </c>
     </row>
@@ -16828,7 +16101,7 @@
         <v>128545</v>
       </c>
       <c r="D88">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>5.1090551886051667</v>
       </c>
     </row>
@@ -16885,7 +16158,7 @@
         <v>1683</v>
       </c>
       <c r="D92">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3.2260841159758238</v>
       </c>
     </row>
@@ -16900,7 +16173,7 @@
         <v>6986</v>
       </c>
       <c r="D93">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3.8442285813016279</v>
       </c>
     </row>
@@ -16915,7 +16188,7 @@
         <v>2864372</v>
       </c>
       <c r="D94">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>6.4570294197307767</v>
       </c>
     </row>
@@ -16930,7 +16203,7 @@
         <v>1365113</v>
       </c>
       <c r="D95">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>6.1351686024721932</v>
       </c>
     </row>
@@ -16945,7 +16218,7 @@
         <v>68758</v>
       </c>
       <c r="D96">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4.8373232356474141</v>
       </c>
     </row>
@@ -16967,4 +16240,146 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D3AFB34-32B6-4BDC-B718-FBEC56218A83}">
+  <dimension ref="F22:I30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F22" sqref="F22:I30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="5.140625" customWidth="1"/>
+    <col min="7" max="7" width="5" customWidth="1"/>
+    <col min="9" max="9" width="7.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="22" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F22" t="s">
+        <v>4</v>
+      </c>
+      <c r="G22" t="s">
+        <v>7</v>
+      </c>
+      <c r="H22" t="s">
+        <v>2</v>
+      </c>
+      <c r="I22" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F23">
+        <v>112</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F24">
+        <v>112</v>
+      </c>
+      <c r="G24">
+        <v>1</v>
+      </c>
+      <c r="H24" s="3">
+        <v>6667</v>
+      </c>
+      <c r="I24" s="6">
+        <f t="shared" ref="I24:I28" si="0">LOG10(H24)</f>
+        <v>3.8239304551255637</v>
+      </c>
+    </row>
+    <row r="25" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F25">
+        <v>112</v>
+      </c>
+      <c r="G25">
+        <v>2</v>
+      </c>
+      <c r="H25" s="3">
+        <v>171203</v>
+      </c>
+      <c r="I25" s="6">
+        <f t="shared" si="0"/>
+        <v>5.2335113705749565</v>
+      </c>
+    </row>
+    <row r="26" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F26">
+        <v>112</v>
+      </c>
+      <c r="G26">
+        <v>3</v>
+      </c>
+      <c r="H26">
+        <v>786338</v>
+      </c>
+      <c r="I26" s="5">
+        <f t="shared" si="0"/>
+        <v>5.8956092635736077</v>
+      </c>
+    </row>
+    <row r="27" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F27">
+        <v>112</v>
+      </c>
+      <c r="G27">
+        <v>4</v>
+      </c>
+      <c r="H27">
+        <v>1397797</v>
+      </c>
+      <c r="I27" s="5">
+        <f t="shared" si="0"/>
+        <v>6.1454441040410508</v>
+      </c>
+    </row>
+    <row r="28" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F28">
+        <v>112</v>
+      </c>
+      <c r="G28">
+        <v>5</v>
+      </c>
+      <c r="H28">
+        <v>284</v>
+      </c>
+      <c r="I28" s="5">
+        <f t="shared" si="0"/>
+        <v>2.4533183400470375</v>
+      </c>
+    </row>
+    <row r="29" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F29">
+        <v>112</v>
+      </c>
+      <c r="G29">
+        <v>6</v>
+      </c>
+      <c r="H29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F30">
+        <v>112</v>
+      </c>
+      <c r="G30">
+        <v>7</v>
+      </c>
+      <c r="H30">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
cleanup prior to full combinatorial run
</commit_message>
<xml_diff>
--- a/Misc/Delta_Individual_Estimates.xlsx
+++ b/Misc/Delta_Individual_Estimates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jorda\Documents\GitHub\VPC\Misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FC5320C-4C7F-4D10-8BBE-8A07CBDD2650}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{416595AF-9A2D-4252-A906-B773273B7267}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{660BBDA3-78F1-466A-B893-49A65C04D429}"/>
+    <workbookView xWindow="13935" yWindow="0" windowWidth="13935" windowHeight="16200" xr2:uid="{660BBDA3-78F1-466A-B893-49A65C04D429}"/>
   </bookViews>
   <sheets>
     <sheet name="δ" sheetId="1" r:id="rId1"/>
@@ -163,7 +163,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -175,7 +175,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -940,9 +939,6 @@
                 <c:pt idx="2">
                   <c:v>6.4900145546065566</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>3.5051499783199058</c:v>
-                </c:pt>
                 <c:pt idx="4">
                   <c:v>7.2797764390576933</c:v>
                 </c:pt>
@@ -1072,9 +1068,6 @@
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>6.4900145546065566</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3.5051499783199058</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>7.2797764390576933</c:v>
@@ -14619,8 +14612,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36985D2A-8E3F-4C08-B816-7EE32E3C5FF0}">
   <dimension ref="A1:Z97"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="U19" sqref="U19"/>
+    <sheetView tabSelected="1" topLeftCell="F31" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="U13" sqref="U13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14909,11 +14902,11 @@
         <v>307</v>
       </c>
       <c r="U12">
-        <v>-0.22739999999999999</v>
+        <v>-0.51970000000000005</v>
       </c>
       <c r="V12">
         <f t="shared" si="1"/>
-        <v>0.52360785014684597</v>
+        <v>1.1966534728290057</v>
       </c>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.25">
@@ -14996,7 +14989,7 @@
         <v>4.3848728944929212</v>
       </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>107</v>
       </c>
@@ -15010,7 +15003,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>110</v>
       </c>
@@ -15026,7 +15019,7 @@
       <c r="U18" s="5"/>
       <c r="V18" s="5"/>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>110</v>
       </c>
@@ -15043,7 +15036,7 @@
       <c r="U19" s="5"/>
       <c r="V19" s="5"/>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>110</v>
       </c>
@@ -15058,7 +15051,7 @@
         <v>5.2335113705749565</v>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>110</v>
       </c>
@@ -15073,7 +15066,7 @@
         <v>5.2518376824661352</v>
       </c>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>110</v>
       </c>
@@ -15081,7 +15074,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>110</v>
       </c>
@@ -15096,7 +15089,7 @@
         <v>3.9674543681827408</v>
       </c>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>110</v>
       </c>
@@ -15110,7 +15103,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>110</v>
       </c>
@@ -15124,7 +15117,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>111</v>
       </c>
@@ -15138,7 +15131,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>111</v>
       </c>
@@ -15152,9 +15145,8 @@
         <f t="shared" si="0"/>
         <v>3.8239304551255637</v>
       </c>
-      <c r="W27" s="7"/>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>111</v>
       </c>
@@ -15168,9 +15160,8 @@
         <f t="shared" si="0"/>
         <v>5.2335113705749565</v>
       </c>
-      <c r="W28" s="7"/>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>111</v>
       </c>
@@ -15185,7 +15176,7 @@
         <v>5.442365300922031</v>
       </c>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>111</v>
       </c>
@@ -15200,7 +15191,7 @@
         <v>4.7160868537748319</v>
       </c>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>111</v>
       </c>
@@ -15215,7 +15206,7 @@
         <v>5.7763226454454557</v>
       </c>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>111</v>
       </c>
@@ -15879,13 +15870,6 @@
       </c>
       <c r="B77">
         <v>3</v>
-      </c>
-      <c r="C77">
-        <v>3200</v>
-      </c>
-      <c r="D77">
-        <f t="shared" si="2"/>
-        <v>3.5051499783199058</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>